<commit_message>
End-of-week T/L, journal  update
Almost done with RecCalc.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-13june2016.xlsx
+++ b/time-labor/week-of-13june2016.xlsx
@@ -35,6 +35,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -133,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Multiple time entries on Friday carried onto Sunday to account for clocking out for seminar</t>
   </si>
   <si>
     <t xml:space="preserve">Sunday</t>
@@ -601,19 +606,19 @@
     <tabColor rgb="FFD9D9D9"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:K27"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="V31" activeCellId="0" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="8.10204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -887,13 +892,17 @@
       <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="19" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D16" s="20" t="n">
+        <v>0.583333333333333</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -907,13 +916,17 @@
       <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.625</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -928,16 +941,16 @@
         <v>28</v>
       </c>
       <c r="C18" s="19" t="n">
-        <v>0</v>
+        <v>0.701388888888889</v>
       </c>
       <c r="D18" s="20" t="n">
-        <v>0</v>
+        <v>0.760416666666667</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>1.41666666666667</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -946,10 +959,13 @@
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
+      <c r="L18" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" s="19" t="n">
         <v>0</v>
@@ -977,11 +993,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>12.5833333333333</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1003,7 +1019,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1025,7 +1041,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>125.833333333333</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1041,7 +1057,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>125.833333333333</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1070,14 +1086,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1090,14 +1106,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>